<commit_message>
- Update file struct - Update doc list
</commit_message>
<xml_diff>
--- a/Перечень документов.xlsx
+++ b/Перечень документов.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990EF2CC-70F6-43F1-B69E-B9B2E356CC2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Общий список" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Таблица с перечнями и критериями отказов для каждого устройства</t>
   </si>
@@ -67,12 +68,24 @@
   </si>
   <si>
     <t>Готовность</t>
+  </si>
+  <si>
+    <t>UML Class Diagram</t>
+  </si>
+  <si>
+    <t>UML Use Case Diagram</t>
+  </si>
+  <si>
+    <t>Class Analysis Diagram</t>
+  </si>
+  <si>
+    <t>IDEF0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -383,20 +396,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="90.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="90.86328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -404,74 +417,94 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Add use case diagram v0.1 - Update other docs - Visual changes on activity diagram and class analysis diagram
</commit_message>
<xml_diff>
--- a/Перечень документов.xlsx
+++ b/Перечень документов.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990EF2CC-70F6-43F1-B69E-B9B2E356CC2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Общий список" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Таблица с перечнями и критериями отказов для каждого устройства</t>
   </si>
@@ -80,12 +79,27 @@
   </si>
   <si>
     <t>IDEF0</t>
+  </si>
+  <si>
+    <t>v0.1</t>
+  </si>
+  <si>
+    <t>v1.0</t>
+  </si>
+  <si>
+    <t>UML Activity Diagram</t>
+  </si>
+  <si>
+    <t>Техническое задание (ГОСТ 34.602-2020)</t>
+  </si>
+  <si>
+    <t>рыба</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -396,20 +410,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="90.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="90.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -417,94 +431,122 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>